<commit_message>
Documentation and mods to filenames etc.
</commit_message>
<xml_diff>
--- a/create-data/_documentation/01. planning/October 30th Brexit data load plan 0.1.xlsx
+++ b/create-data/_documentation/01. planning/October 30th Brexit data load plan 0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/_documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/_documentation/01. planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B8C77B-97EA-D64E-8F87-46B874CC8CCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5B6D6D-EF39-D149-8EEE-690B61C6E48B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7420" yWindow="820" windowWidth="22600" windowHeight="17640" xr2:uid="{70EE06A5-C50A-4690-B6BE-3CA10D1D3B38}"/>
   </bookViews>
@@ -483,17 +483,6 @@
     <t>python3 convert.py TGB19062.xml quotas_wto10.xml</t>
   </si>
   <si>
-    <t>python3 migrate_measures.py r r trade_remedies3</t>
-  </si>
-  <si>
-    <t>python3 migrate_measures.py r r trade_remedies4</t>
-  </si>
-  <si>
-    <t>python3 migrate_measures.py m t cred N1234567
-python3 migrate_measures.py m r supp I1900010
-python3 migrate_measures.py m t cred N1234567</t>
-  </si>
-  <si>
     <t>python3 migrate_measures.py m t wto_quotas N1234567</t>
   </si>
   <si>
@@ -625,15 +614,25 @@
     <t>python3 commodities.py</t>
   </si>
   <si>
-    <t>python3 kill_all_quota_definitions.py</t>
-  </si>
-  <si>
-    <t>python3 base_regulations.py gsp
-python3 migrate_measures.py r t R120978
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>python3 migrate_measures.py m t cred
+python3 migrate_measures.py m r supp I1900010
+python3 migrate_measures.py m t surv</t>
+  </si>
+  <si>
+    <t>python3 migrate_measures.py r r profile_trade_remedies1</t>
+  </si>
+  <si>
+    <t>python3 migrate_measures.py r r profile_trade_remedies2</t>
+  </si>
+  <si>
+    <t>python3 migrate_measures.py r t R120978
 python3 gsp.py 2020</t>
   </si>
   <si>
-    <t>Documentation</t>
+    <t>python3 terminate_quota_definitions.py</t>
   </si>
 </sst>
 </file>
@@ -1116,11 +1115,11 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="109" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>9</v>
@@ -2421,7 +2420,7 @@
         <v>18</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>63</v>
@@ -2450,7 +2449,7 @@
         <v>19</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="L40" s="9" t="s">
         <v>64</v>
@@ -2479,7 +2478,7 @@
         <v>20</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="L41" s="9" t="s">
         <v>65</v>
@@ -2512,7 +2511,7 @@
         <v>22</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="L42" s="9" t="s">
         <v>66</v>
@@ -2545,7 +2544,7 @@
         <v>23</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L43" s="9" t="s">
         <v>67</v>
@@ -2578,7 +2577,7 @@
         <v>25</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L44" s="9" t="s">
         <v>68</v>
@@ -2611,7 +2610,7 @@
         <v>26</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L45" s="9" t="s">
         <v>69</v>
@@ -2644,7 +2643,7 @@
         <v>27</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L46" s="9" t="s">
         <v>70</v>
@@ -2675,7 +2674,7 @@
         <v>29</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L47" s="9" t="s">
         <v>71</v>
@@ -2706,7 +2705,7 @@
         <v>30</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L48" s="9" t="s">
         <v>72</v>
@@ -2737,7 +2736,7 @@
         <v>31</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L49" s="9" t="s">
         <v>73</v>
@@ -2767,7 +2766,7 @@
         <v>32</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L50" s="9" t="s">
         <v>74</v>
@@ -2797,7 +2796,7 @@
         <v>33</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L51" s="9" t="s">
         <v>75</v>
@@ -2827,7 +2826,7 @@
         <v>34</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L52" s="9" t="s">
         <v>76</v>
@@ -2857,13 +2856,13 @@
         <v>35</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L53" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="36" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>43557</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>36</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L55" s="9" t="s">
         <v>79</v>
@@ -2946,7 +2945,7 @@
         <v>37</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L56" s="9" t="s">
         <v>80</v>
@@ -2975,7 +2974,7 @@
         <v>38</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L57" s="9" t="s">
         <v>81</v>
@@ -3004,7 +3003,7 @@
         <v>39</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L58" s="9" t="s">
         <v>82</v>
@@ -3039,7 +3038,7 @@
         <v>40</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L59" s="9" t="s">
         <v>84</v>
@@ -3074,7 +3073,7 @@
         <v>41</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L60" s="9" t="s">
         <v>86</v>
@@ -3103,7 +3102,7 @@
         <v>60</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L61" s="9" t="s">
         <v>87</v>
@@ -3129,7 +3128,7 @@
         <v>42</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L62" s="9" t="s">
         <v>88</v>
@@ -3155,7 +3154,7 @@
         <v>43</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L63" s="9" t="s">
         <v>89</v>
@@ -3187,7 +3186,7 @@
         <v>44</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L64" s="9" t="s">
         <v>91</v>
@@ -3219,7 +3218,7 @@
         <v>45</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L65" s="9" t="s">
         <v>93</v>
@@ -3251,7 +3250,7 @@
         <v>46</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L66" s="9" t="s">
         <v>95</v>
@@ -3283,7 +3282,7 @@
         <v>56</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L67" s="9" t="s">
         <v>97</v>
@@ -3312,7 +3311,7 @@
         <v>47</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L68" s="9" t="s">
         <v>99</v>
@@ -3344,7 +3343,7 @@
         <v>48</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L69" s="9" t="s">
         <v>101</v>
@@ -3376,7 +3375,7 @@
         <v>49</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L70" s="9" t="s">
         <v>103</v>
@@ -3408,7 +3407,7 @@
         <v>50</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L71" s="9" t="s">
         <v>105</v>
@@ -3434,7 +3433,7 @@
         <v>51</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L72" s="9" t="s">
         <v>107</v>
@@ -3451,7 +3450,7 @@
         <v>59</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L73" s="9" t="s">
         <v>108</v>
@@ -3468,7 +3467,7 @@
         <v>61</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L74" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Documentation for quota migration
</commit_message>
<xml_diff>
--- a/create-data/_documentation/01. planning/October 30th Brexit data load plan 0.1.xlsx
+++ b/create-data/_documentation/01. planning/October 30th Brexit data load plan 0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/_documentation/01. planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5B6D6D-EF39-D149-8EEE-690B61C6E48B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE034D0-8250-224E-A0CF-7342B61EDD5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7420" yWindow="820" windowWidth="22600" windowHeight="17640" xr2:uid="{70EE06A5-C50A-4690-B6BE-3CA10D1D3B38}"/>
   </bookViews>
@@ -483,9 +483,6 @@
     <t>python3 convert.py TGB19062.xml quotas_wto10.xml</t>
   </si>
   <si>
-    <t>python3 migrate_measures.py m t wto_quotas N1234567</t>
-  </si>
-  <si>
     <t>python3 migrate_measures.py c t mexico N1234567
 python3 migrate_measures.py c t jordan N1234567
 python3 migrate_measures.py c t moldova N1234567
@@ -633,6 +630,9 @@
   </si>
   <si>
     <t>python3 terminate_quota_definitions.py</t>
+  </si>
+  <si>
+    <t>python3 migrate_measures.py m t quotas</t>
   </si>
 </sst>
 </file>
@@ -1115,11 +1115,11 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="109" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-      <selection pane="bottomRight" activeCell="J44" sqref="J44"/>
+      <selection pane="bottomRight" activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>9</v>
@@ -2420,7 +2420,7 @@
         <v>18</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>63</v>
@@ -2449,7 +2449,7 @@
         <v>19</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L40" s="9" t="s">
         <v>64</v>
@@ -2478,7 +2478,7 @@
         <v>20</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L41" s="9" t="s">
         <v>65</v>
@@ -2511,7 +2511,7 @@
         <v>22</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L42" s="9" t="s">
         <v>66</v>
@@ -2544,7 +2544,7 @@
         <v>23</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L43" s="9" t="s">
         <v>67</v>
@@ -2577,7 +2577,7 @@
         <v>25</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="L44" s="9" t="s">
         <v>68</v>
@@ -2610,7 +2610,7 @@
         <v>26</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L45" s="9" t="s">
         <v>69</v>
@@ -2643,7 +2643,7 @@
         <v>27</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L46" s="9" t="s">
         <v>70</v>
@@ -2674,7 +2674,7 @@
         <v>29</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L47" s="9" t="s">
         <v>71</v>
@@ -2705,7 +2705,7 @@
         <v>30</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L48" s="9" t="s">
         <v>72</v>
@@ -2736,7 +2736,7 @@
         <v>31</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L49" s="9" t="s">
         <v>73</v>
@@ -2766,7 +2766,7 @@
         <v>32</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L50" s="9" t="s">
         <v>74</v>
@@ -2796,7 +2796,7 @@
         <v>33</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L51" s="9" t="s">
         <v>75</v>
@@ -2826,7 +2826,7 @@
         <v>34</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L52" s="9" t="s">
         <v>76</v>
@@ -2856,7 +2856,7 @@
         <v>35</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L53" s="9" t="s">
         <v>77</v>
@@ -2886,7 +2886,7 @@
         <v>58</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L54" s="9" t="s">
         <v>78</v>
@@ -2916,7 +2916,7 @@
         <v>36</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L55" s="9" t="s">
         <v>79</v>
@@ -2945,7 +2945,7 @@
         <v>37</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L56" s="9" t="s">
         <v>80</v>
@@ -2974,7 +2974,7 @@
         <v>38</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L57" s="9" t="s">
         <v>81</v>
@@ -3003,7 +3003,7 @@
         <v>39</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L58" s="9" t="s">
         <v>82</v>
@@ -3038,7 +3038,7 @@
         <v>40</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L59" s="9" t="s">
         <v>84</v>
@@ -3073,7 +3073,7 @@
         <v>41</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L60" s="9" t="s">
         <v>86</v>
@@ -3102,7 +3102,7 @@
         <v>60</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L61" s="9" t="s">
         <v>87</v>
@@ -3128,7 +3128,7 @@
         <v>42</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L62" s="9" t="s">
         <v>88</v>
@@ -3154,7 +3154,7 @@
         <v>43</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L63" s="9" t="s">
         <v>89</v>
@@ -3186,7 +3186,7 @@
         <v>44</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L64" s="9" t="s">
         <v>91</v>
@@ -3218,7 +3218,7 @@
         <v>45</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L65" s="9" t="s">
         <v>93</v>
@@ -3250,7 +3250,7 @@
         <v>46</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L66" s="9" t="s">
         <v>95</v>
@@ -3282,7 +3282,7 @@
         <v>56</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L67" s="9" t="s">
         <v>97</v>
@@ -3311,7 +3311,7 @@
         <v>47</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L68" s="9" t="s">
         <v>99</v>
@@ -3343,7 +3343,7 @@
         <v>48</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L69" s="9" t="s">
         <v>101</v>
@@ -3375,7 +3375,7 @@
         <v>49</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L70" s="9" t="s">
         <v>103</v>
@@ -3407,7 +3407,7 @@
         <v>50</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L71" s="9" t="s">
         <v>105</v>
@@ -3433,7 +3433,7 @@
         <v>51</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L72" s="9" t="s">
         <v>107</v>
@@ -3450,7 +3450,7 @@
         <v>59</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L73" s="9" t="s">
         <v>108</v>
@@ -3467,7 +3467,7 @@
         <v>61</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L74" s="9" t="s">
         <v>109</v>

</xml_diff>